<commit_message>
Minor fix in ps table
</commit_message>
<xml_diff>
--- a/development/L1Menu_Collisions2023_v1_0_0/PrescaleTable/L1Menu_Collisions2023_v1_0_0.xlsx
+++ b/development/L1Menu_Collisions2023_v1_0_0/PrescaleTable/L1Menu_Collisions2023_v1_0_0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caterinaaruta/Desktop/L1Menus/L1Menu_Collisions2023_v1_0_0/PrescaleTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38D330C7-7A16-EE4F-8D56-4032E84D0516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D8F403-450C-C34E-976E-8F017750C188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3140" yWindow="-18140" windowWidth="31160" windowHeight="18140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3420" yWindow="-18140" windowWidth="31160" windowHeight="18140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="(L1Menu_Collisions2022_v1_3_0 -" sheetId="1" r:id="rId1"/>
@@ -1639,10 +1639,10 @@
   <dimension ref="A1:AB1006"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C114" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I31" sqref="I31"/>
+      <selection pane="bottomRight" activeCell="G139" sqref="G139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -10639,28 +10639,28 @@
         <v>0</v>
       </c>
       <c r="D139" s="5">
-        <v>1500</v>
+        <v>1550</v>
       </c>
       <c r="E139" s="5">
-        <v>1500</v>
+        <v>1550</v>
       </c>
       <c r="F139" s="5">
-        <v>1500</v>
+        <v>1550</v>
       </c>
       <c r="G139" s="5">
-        <v>1500</v>
+        <v>1550</v>
       </c>
       <c r="H139" s="5">
-        <v>1500</v>
+        <v>1550</v>
       </c>
       <c r="I139" s="5">
-        <v>1500</v>
+        <v>1550</v>
       </c>
       <c r="J139" s="5">
-        <v>1500</v>
+        <v>1550</v>
       </c>
       <c r="K139" s="5">
-        <v>1500</v>
+        <v>1550</v>
       </c>
       <c r="L139" s="5">
         <v>775</v>

</xml_diff>

<commit_message>
Minor update in PS table (L1_SingleJet60_FWD2p5)
</commit_message>
<xml_diff>
--- a/development/L1Menu_Collisions2023_v1_0_0/PrescaleTable/L1Menu_Collisions2023_v1_0_0.xlsx
+++ b/development/L1Menu_Collisions2023_v1_0_0/PrescaleTable/L1Menu_Collisions2023_v1_0_0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caterinaaruta/Desktop/L1Menus/L1Menu_Collisions2023_v1_0_0/PrescaleTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17C528C1-8D38-1347-93ED-3E0232B94E1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C80F9A78-F831-9D4E-AA30-6F0EE6622E2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28800" windowHeight="16680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="(L1Menu_Collisions2022_v1_3_0 -" sheetId="1" r:id="rId1"/>
@@ -1657,10 +1657,10 @@
   <dimension ref="A1:AB1012"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C260" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomRight" activeCell="C292" sqref="C292"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -19952,58 +19952,58 @@
         <v>0</v>
       </c>
       <c r="D282" s="5">
-        <v>5461</v>
+        <v>1820</v>
       </c>
       <c r="E282" s="5">
-        <v>5461</v>
+        <v>1820</v>
       </c>
       <c r="F282" s="5">
-        <v>5461</v>
+        <v>1820</v>
       </c>
       <c r="G282" s="5">
-        <v>5461</v>
+        <v>1820</v>
       </c>
       <c r="H282" s="5">
-        <v>5461</v>
+        <v>1820</v>
       </c>
       <c r="I282" s="5">
-        <v>5461</v>
+        <v>1820</v>
       </c>
       <c r="J282" s="5">
-        <v>5461</v>
+        <v>1820</v>
       </c>
       <c r="K282" s="5">
-        <v>5461</v>
+        <v>1820</v>
       </c>
       <c r="L282" s="5">
-        <v>5461</v>
+        <v>1820</v>
       </c>
       <c r="M282" s="5">
-        <v>5461</v>
+        <v>1820</v>
       </c>
       <c r="N282" s="5">
-        <v>5461</v>
+        <v>1820</v>
       </c>
       <c r="O282" s="5">
-        <v>5461</v>
+        <v>1820</v>
       </c>
       <c r="P282" s="5">
-        <v>5461</v>
+        <v>1820</v>
       </c>
       <c r="Q282" s="5">
-        <v>5461</v>
+        <v>1820</v>
       </c>
       <c r="R282" s="5">
-        <v>5461</v>
+        <v>1820</v>
       </c>
       <c r="S282" s="5">
-        <v>5461</v>
+        <v>1820</v>
       </c>
       <c r="T282" s="5">
-        <v>5461</v>
+        <v>1820</v>
       </c>
       <c r="U282" s="5">
-        <v>5461</v>
+        <v>1820</v>
       </c>
     </row>
     <row r="283" spans="1:21" ht="13" x14ac:dyDescent="0.15">
@@ -41233,17 +41233,17 @@
       <c r="U1012" s="5"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D247:U253 C125:C253 D125:U245 C254:U416 C2:U124">
+  <conditionalFormatting sqref="D247:U253 C125:C253 D125:U245 C2:U124 C254:U416">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D247:U253 C125:C253 D125:U245 C254:U416 C2:U124">
+  <conditionalFormatting sqref="D247:U253 C125:C253 D125:U245 C2:U124 C254:U416">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D247:U253 C125:C253 D125:U245 C254:U416 C2:U124">
+  <conditionalFormatting sqref="D247:U253 C125:C253 D125:U245 C2:U124 C254:U416">
     <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
       <formula>1</formula>
     </cfRule>

</xml_diff>